<commit_message>
I've completed the BOM for version 1 of the PCB for the reflector. Regarding the board and schematic themselves, the board needs to be mapped out with all parts oriented before being reviewed.
</commit_message>
<xml_diff>
--- a/reflector/BOM/Handheld Ground Station BOM.xlsx
+++ b/reflector/BOM/Handheld Ground Station BOM.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4760" yWindow="460" windowWidth="20840" windowHeight="14580" tabRatio="500"/>
+    <workbookView xWindow="22400" yWindow="580" windowWidth="15100" windowHeight="19640" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="77">
   <si>
     <t>LP2985-33DBVR</t>
   </si>
@@ -71,9 +71,6 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>AR9271</t>
-  </si>
-  <si>
     <t>https://www.datasheetq.com/AR9271-doc-Qualcomm</t>
   </si>
   <si>
@@ -89,9 +86,6 @@
     <t>USB 2.0 cable</t>
   </si>
   <si>
-    <t>Mnf</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -134,11 +128,140 @@
     <t xml:space="preserve">2.7GHz, 5.25V, 8-Pin DFN </t>
   </si>
   <si>
-    <t>772-TQP3M9037-PCB</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 772-QPQ1907EVB01
+    <t>Mnf.</t>
+  </si>
+  <si>
+    <t>Digi-Key</t>
+  </si>
+  <si>
+    <t>713-110991027</t>
+  </si>
+  <si>
+    <t>L71532-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4304H1 </t>
+  </si>
+  <si>
+    <t>VCC</t>
+  </si>
+  <si>
+    <t>LED1</t>
+  </si>
+  <si>
+    <t>PI_USB_OUT</t>
+  </si>
+  <si>
+    <t>AR9721</t>
+  </si>
+  <si>
+    <t>U$4</t>
+  </si>
+  <si>
+    <t>Aliexpress</t>
+  </si>
+  <si>
+    <t>296-18476-2-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">772-QPQ1907EVB01
 </t>
+  </si>
+  <si>
+    <t>Molex</t>
+  </si>
+  <si>
+    <t>772-TQP3M9037</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/Search/Refine?N=4282285770&amp;Keyword=772-TQP3M9037&amp;utm_source=octopart&amp;utm_medium=aggregator&amp;utm_campaign=772-TQP3M9037&amp;utm_content=Qorvo</t>
+  </si>
+  <si>
+    <t>Source file: HGS_reflector.sch</t>
+  </si>
+  <si>
+    <t>BOM version: 1</t>
+  </si>
+  <si>
+    <t>PCB version: 2.0</t>
+  </si>
+  <si>
+    <t>R9</t>
+  </si>
+  <si>
+    <t>2 kOhms ±2%, xW</t>
+  </si>
+  <si>
+    <t>C1, C3, C4, C11, C14</t>
+  </si>
+  <si>
+    <t>C9</t>
+  </si>
+  <si>
+    <t>C8</t>
+  </si>
+  <si>
+    <t>C2, C5, C12</t>
+  </si>
+  <si>
+    <t>Panasonic</t>
+  </si>
+  <si>
+    <t>KEMET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  CAN12C103KAGACTU</t>
+  </si>
+  <si>
+    <t>80-CAN12C103KAGACTU</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/KEMET/CAN12C103KAGACTU?qs=sGAEpiMZZMsh%252B1woXyUXj9e2R%2FOkAO5o%252BI3tG6%2FoqZA%3D</t>
+  </si>
+  <si>
+    <t>80-R60DF4220506AK</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/KEMET/R60DF4220506AK?qs=MdJgNetHbflDvWJrlNhA6Q%3D%3D</t>
+  </si>
+  <si>
+    <t>Completion Date: 8/20/20</t>
+  </si>
+  <si>
+    <t>100 pF ± 5%, length: 5mm, 40VAC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+PFR5101J63J11L4BULK</t>
+  </si>
+  <si>
+    <t>80-PFR5101J63J11L4</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/KEMET/PFR5101J63J11L4BULK?qs=RAUrRqLvb8x%252BXbF4f8QHtA%3D%3D</t>
+  </si>
+  <si>
+    <t>1uF ± 5%, length: 7.5 mm, 40VAC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R66DD4100Z37AJ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+80-R66DD4100Z37AJ</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/KEMET/R66DD4100Z37AJ?qs=pfd5qewlna6qVtDxM97tlQ%3D%3D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+R60DF4220506AK </t>
+  </si>
+  <si>
+    <t>10nF ± 10%, length: 3.5 mm, 250VAC</t>
+  </si>
+  <si>
+    <t>2.2uF ± 10%, length: 13mm, 40VAC</t>
   </si>
 </sst>
 </file>
@@ -180,7 +303,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -189,6 +312,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -466,208 +593,406 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.42578125" customWidth="1"/>
-    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" customWidth="1"/>
-    <col min="5" max="5" width="46" customWidth="1"/>
-    <col min="8" max="8" width="17.5703125" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" customWidth="1"/>
+    <col min="8" max="8" width="22.85546875" customWidth="1"/>
     <col min="9" max="9" width="64.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="B1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="70" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I1" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="70" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="36" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" t="s">
-        <v>33</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="I3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" t="s">
-        <v>26</v>
-      </c>
-      <c r="I5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" t="s">
-        <v>25</v>
-      </c>
-      <c r="I6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="54" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
-      <c r="C7" t="s">
-        <v>19</v>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="54" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
       <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="H8" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H9" t="s">
+        <v>35</v>
+      </c>
+      <c r="I9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" t="s">
+        <v>43</v>
+      </c>
+      <c r="H10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" t="s">
         <v>34</v>
       </c>
-      <c r="D8" t="s">
+      <c r="H11" t="s">
+        <v>36</v>
+      </c>
+      <c r="I11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" t="s">
+        <v>46</v>
+      </c>
+      <c r="H12" s="3">
+        <v>887329220</v>
+      </c>
+      <c r="I12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="54" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="D13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8" t="s">
-        <v>33</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>35</v>
+      <c r="F13" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" t="s">
+        <v>31</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14" t="s">
+        <v>23</v>
+      </c>
+      <c r="I14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="36" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>4</v>
+      </c>
+      <c r="B15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F15" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" t="s">
+        <v>31</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="36" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D16" t="s">
+        <v>71</v>
+      </c>
+      <c r="E16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F16" t="s">
+        <v>23</v>
+      </c>
+      <c r="G16" t="s">
+        <v>31</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="36" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E17" t="s">
+        <v>59</v>
+      </c>
+      <c r="F17" t="s">
+        <v>23</v>
+      </c>
+      <c r="G17" t="s">
+        <v>31</v>
+      </c>
+      <c r="H17" t="s">
+        <v>63</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="36" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D18" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" t="s">
+        <v>59</v>
+      </c>
+      <c r="F18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G18" t="s">
+        <v>31</v>
+      </c>
+      <c r="H18" t="s">
+        <v>61</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>